<commit_message>
added tables: tasks, things, associations
</commit_message>
<xml_diff>
--- a/datasets/objects.xlsx
+++ b/datasets/objects.xlsx
@@ -426,7 +426,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D12"/>
+  <dimension ref="A1:D13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -651,6 +651,24 @@
       <c r="D12" t="inlineStr">
         <is>
           <t>Surface Book 3</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="1" t="inlineStr">
+        <is>
+          <t>8f4a9a29-4edd-4c6b-8214-306c3778ab4a</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>12/10/2022</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr"/>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>Vehicle Logistics Trainee</t>
         </is>
       </c>
     </row>

</xml_diff>